<commit_message>
replace quotes in description
</commit_message>
<xml_diff>
--- a/molgenis-model-registry/src/test/resources/PhenDB/PhenDB_DBMP/PhenDB_DBMP.xlsx
+++ b/molgenis-model-registry/src/test/resources/PhenDB/PhenDB_DBMP/PhenDB_DBMP.xlsx
@@ -1831,8 +1831,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1907,7 +1909,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1939,6 +1941,7 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1970,6 +1973,7 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>

</xml_diff>